<commit_message>
Creation of Components folder
</commit_message>
<xml_diff>
--- a/Tier System/in progress/v02-10/NBO-Microscopy Metadata Tier System_v02-10.xlsx
+++ b/Tier System/in progress/v02-10/NBO-Microscopy Metadata Tier System_v02-10.xlsx
@@ -8,21 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/strambc/Documents/GitHub/NBOMicroscopyMetadataSpecs/Tier System/in progress/v02-10/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2E3C365-8C73-A545-9AC5-833001446690}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{739C4A4A-C770-A844-9BF8-51BBAF984BB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31860" yWindow="1940" windowWidth="28400" windowHeight="20060" tabRatio="914" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27920" windowHeight="16820" tabRatio="914" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tier system_v02-10" sheetId="12" r:id="rId1"/>
+    <sheet name="Tier system_v02-10_NBO SupTab I" sheetId="12" r:id="rId1"/>
     <sheet name="Tier system_v02-10 SUMMARY_1" sheetId="13" r:id="rId2"/>
     <sheet name="Tier system_v02-10 SUMMARY 2" sheetId="14" r:id="rId3"/>
-    <sheet name="Tier system_v02-10 MINIMAL" sheetId="16" r:id="rId4"/>
+    <sheet name="Tier system_v02-10_NBO Table I" sheetId="17" r:id="rId4"/>
+    <sheet name="Tier system_v02-10 MINIMAL" sheetId="16" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Tier system_v02-10'!$A$2:$L$5</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="3">'Tier system_v02-10 MINIMAL'!$A$2:$B$5</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">'Tier system_v02-10 MINIMAL'!$A$2:$B$5</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">'Tier system_v02-10 SUMMARY 2'!$A$2:$H$5</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'Tier system_v02-10 SUMMARY_1'!$A$1:$J$5</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'Tier system_v02-10 SUMMARY_1'!$A$1:$J$4</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Tier system_v02-10_NBO SupTab I'!$A$2:$L$6</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">'Tier system_v02-10_NBO Table I'!$A$1:$E$6</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="58">
   <si>
     <t>Name</t>
   </si>
@@ -96,20 +98,10 @@
 Full Documentation</t>
   </si>
   <si>
-    <t>Minimum Information/  
-Material &amp; Methods</t>
-  </si>
-  <si>
     <t>Reporting qualitative effects, or effects that require simple quantification including the identification of non-refractive limited objects followed by basic  feature extraction and statistical analysis</t>
   </si>
   <si>
     <t>Full documentation of microscopic setup, image acquisition and quality control</t>
-  </si>
-  <si>
-    <t>Diffraction-limited spot localization, measurement of distances, co-localization studies, signal-starved features, advanced processing, cell tracking and single-particle tracking, dynamic expression level quantification</t>
-  </si>
-  <si>
-    <t>Microscopy hardware manufacturing;  development of novel unproven technology in both commercial and academic settings; full reproducibility of microscopy set-up and image acquisition settings</t>
   </si>
   <si>
     <t>All of the above +  Single Molecule (SM) FISH, CasFISH, SM Proximity Ligation Assay (PLA), dCas9-based labelling, OligoPaint</t>
@@ -168,12 +160,6 @@
   </si>
   <si>
     <t>Example Experiment Type</t>
-  </si>
-  <si>
-    <t>Reporting qualitative effects, or effects that require simple quantification including the identification of objects larger than the resolution limit followed by basic  feature extraction and statistical analysis</t>
-  </si>
-  <si>
-    <t>Supplemental Table I</t>
   </si>
   <si>
     <t>detailed environmental control device, microscope table, light source, light source coupling, transmittance light path,  magnification, sample positioning, focusing,  autofocus, filter, dichroic, additional optics and detector specification (e.g., lightsource spectral properties; objective correction properties; focusing device ZReproducibility, ZSettlingTime, ZResolution, etc.)</t>
@@ -206,34 +192,69 @@
     </r>
   </si>
   <si>
+    <t>Advanced Quantification</t>
+  </si>
+  <si>
+    <t>Developmental and stem-biology experiments in which qualitative analysis of image data is used to support major findings, transfection control, viability assay, counting of cells and nuclei, expression level measurements, localization of markers in cellular sub-compartments</t>
+  </si>
+  <si>
+    <t>Reporting quantitative effects that require advanced quantification including the localization of single molecules and  tracking of intracellular dynamics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Table I: Tiers for light microscopy metadata reporting as proposed by the Imaging Standards Working Group of the 4D Nucleome initiative and by the Quality Control and Data Management Working Group of Bioimaging North America. </t>
+  </si>
+  <si>
+    <t>Nr.</t>
+  </si>
+  <si>
+    <t>Example</t>
+  </si>
+  <si>
+    <t>Manufacturing/
+Technical Development/
+Full Documentation</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">Manufacturing/ Technical Development: </t>
+      <t xml:space="preserve">Legend: </t>
     </r>
     <r>
       <rPr>
-        <sz val="24"/>
-        <color theme="0"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Full documentation of microscopic setup, image acquisition and quality control</t>
+      <t>Each tier accommodates increasingly complex images, experiments, instrumentation, and analytical needs and therefore requires progressively more metadata. This tiered system is not intended to meet the needs of all imaging communities.  Rather it is proposed as a framework that might need to be adapted and modified depending on the needs of individual data collection consortia, disciplines, or institutions.</t>
     </r>
+  </si>
+  <si>
+    <t>Diffraction-limited spot localization, measurement of distances, co-localization studies, detection of low-signal features, advanced processing, cell tracking and single-particle tracking, dynamic expression level quantification</t>
+  </si>
+  <si>
+    <t>Microscopy hardware manufacturing;  development of novel and yet to be validated technology in both commercial and academic settings; full reproducibility of microscopy set-up and image acquisition settings</t>
+  </si>
+  <si>
+    <t>Minimum Information/ Qualitative or Basic Quantification/
+Material &amp; Methods</t>
+  </si>
+  <si>
+    <t>Reporting quantitative effects that require advanced quantification including the localization of single molecules and tracking of intracellular dynamics</t>
   </si>
   <si>
     <r>
       <rPr>
         <b/>
-        <sz val="24"/>
+        <sz val="23"/>
         <color theme="1"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t>Minimum Information/  
-Material &amp; Methods:</t>
+      <t>Minimum Information/ Qualitative or Basic Quantification/Material &amp; Methods:</t>
     </r>
     <r>
       <rPr>
-        <sz val="24"/>
+        <sz val="23"/>
         <color theme="1"/>
         <rFont val="Arial"/>
         <family val="2"/>
@@ -242,22 +263,10 @@
     </r>
   </si>
   <si>
-    <t>Advanced Quantification</t>
-  </si>
-  <si>
-    <t>Developmental and stem-biology experiments in which qualitative analysis of image data is used to support major findings, transfection control, viability assay, counting of cells and nuclei, expression level measurements, localization of markers in cellular sub-compartments</t>
-  </si>
-  <si>
-    <t>Hystochemistry, Immuno-Hystochemistry,  Fluorescent In Situ Hybridization (FISH), Immuno Fluorescence (IF), Fluoresent Protein (FP) labelling</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Advanced Quantification </t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
-        <sz val="24"/>
+        <sz val="23"/>
         <color theme="1"/>
         <rFont val="Arial"/>
         <family val="2"/>
@@ -266,7 +275,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="24"/>
+        <sz val="23"/>
         <color theme="1"/>
         <rFont val="Arial"/>
         <family val="2"/>
@@ -275,14 +284,28 @@
     </r>
   </si>
   <si>
-    <t>Reporting quantitative effects that require advanced quantification including the localization of single molecules and  tracking of intracellular dynamics</t>
+    <r>
+      <t xml:space="preserve">Manufacturing/ Technical Development: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="23"/>
+        <color theme="0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Full documentation of microscopic setup, image acquisition and quality control</t>
+    </r>
+  </si>
+  <si>
+    <t>Histochemistry, Immuno-Histochemistry,  Fluorescent In Situ Hybridization (FISH), Immuno Fluorescence (IF), Fluorescent Protein (FP) labelling</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="43" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -447,13 +470,124 @@
     </font>
     <font>
       <b/>
-      <sz val="24"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="0"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="23"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="23"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="23"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="23"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -478,8 +612,32 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4CBB9D"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF9038"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0072B2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="26">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -663,17 +821,6 @@
       </top>
       <bottom style="thick">
         <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color theme="1"/>
-      </top>
-      <bottom style="medium">
-        <color theme="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -785,6 +932,37 @@
       </top>
       <bottom style="thin">
         <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -826,7 +1004,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -880,18 +1058,12 @@
     <xf numFmtId="0" fontId="12" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -907,24 +1079,9 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="15" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -949,21 +1106,21 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
@@ -979,25 +1136,13 @@
     <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1009,86 +1154,176 @@
     <xf numFmtId="0" fontId="18" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="12" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="15" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="27" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="35">
@@ -1481,207 +1716,206 @@
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView zoomScale="35" zoomScaleNormal="53" zoomScalePageLayoutView="50" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="29" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="19.5" style="3" customWidth="1"/>
     <col min="2" max="2" width="12" style="1" customWidth="1"/>
-    <col min="3" max="3" width="35.5" style="4" customWidth="1"/>
+    <col min="3" max="3" width="36.83203125" style="4" customWidth="1"/>
     <col min="4" max="4" width="48" style="13" customWidth="1"/>
     <col min="5" max="5" width="67.1640625" style="13" customWidth="1"/>
     <col min="6" max="6" width="55" style="13" customWidth="1"/>
     <col min="7" max="7" width="39.6640625" style="14" customWidth="1"/>
     <col min="8" max="8" width="77.6640625" style="14" customWidth="1"/>
     <col min="9" max="9" width="71.5" style="13" customWidth="1"/>
-    <col min="10" max="11" width="23.6640625" style="13" customWidth="1"/>
-    <col min="12" max="12" width="27.83203125" style="13" customWidth="1"/>
+    <col min="10" max="12" width="23.6640625" style="13" customWidth="1"/>
     <col min="13" max="16384" width="10.83203125" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="127" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="76" t="s">
-        <v>45</v>
-      </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="76"/>
-      <c r="H1" s="76"/>
-      <c r="I1" s="76"/>
-      <c r="J1" s="76"/>
-      <c r="K1" s="76"/>
-      <c r="L1" s="76"/>
-    </row>
-    <row r="2" spans="1:13" s="21" customFormat="1" ht="80" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="42" t="s">
+      <c r="A1" s="91" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="91"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="91"/>
+      <c r="G1" s="91"/>
+      <c r="H1" s="91"/>
+      <c r="I1" s="91"/>
+      <c r="J1" s="91"/>
+      <c r="K1" s="91"/>
+      <c r="L1" s="91"/>
+    </row>
+    <row r="2" spans="1:13" s="20" customFormat="1" ht="80" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="44" t="s">
+      <c r="C2" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="45" t="s">
+      <c r="D2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="F2" s="45" t="s">
+      <c r="E2" s="38" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="45" t="s">
+      <c r="G2" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="L2" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="M2" s="19"/>
+    </row>
+    <row r="3" spans="1:13" s="9" customFormat="1" ht="369" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="22">
+        <v>1</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="69" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="69" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" s="69" t="s">
+        <v>57</v>
+      </c>
+      <c r="G3" s="70" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" s="70" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" s="70" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3" s="69" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" s="95" t="s">
+        <v>33</v>
+      </c>
+      <c r="L3" s="96"/>
+      <c r="M3" s="12"/>
+    </row>
+    <row r="4" spans="1:13" s="10" customFormat="1" ht="406" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="92" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="49">
+        <v>2</v>
+      </c>
+      <c r="C4" s="50" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="71" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="71" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="72" t="s">
         <v>29</v>
       </c>
-      <c r="H2" s="45" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" s="45" t="s">
-        <v>10</v>
-      </c>
-      <c r="J2" s="45" t="s">
+      <c r="H4" s="73" t="s">
+        <v>38</v>
+      </c>
+      <c r="I4" s="74" t="s">
+        <v>31</v>
+      </c>
+      <c r="J4" s="71" t="s">
+        <v>9</v>
+      </c>
+      <c r="K4" s="97" t="s">
+        <v>21</v>
+      </c>
+      <c r="L4" s="98"/>
+      <c r="M4" s="6"/>
+    </row>
+    <row r="5" spans="1:13" s="11" customFormat="1" ht="343" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="92"/>
+      <c r="B5" s="43">
         <v>3</v>
       </c>
-      <c r="K2" s="45" t="s">
-        <v>4</v>
-      </c>
-      <c r="L2" s="45" t="s">
-        <v>8</v>
-      </c>
-      <c r="M2" s="20"/>
-    </row>
-    <row r="3" spans="1:13" s="9" customFormat="1" ht="369" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="24">
-        <v>1</v>
-      </c>
-      <c r="C3" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="31" t="s">
+      <c r="C5" s="44" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="75" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="31" t="s">
-        <v>50</v>
-      </c>
-      <c r="F3" s="31" t="s">
+      <c r="E5" s="75" t="s">
         <v>51</v>
       </c>
-      <c r="G3" s="32" t="s">
-        <v>31</v>
-      </c>
-      <c r="H3" s="32" t="s">
-        <v>30</v>
-      </c>
-      <c r="I3" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="J3" s="31" t="s">
-        <v>35</v>
-      </c>
-      <c r="K3" s="80" t="s">
-        <v>36</v>
-      </c>
-      <c r="L3" s="81"/>
-      <c r="M3" s="12"/>
-    </row>
-    <row r="4" spans="1:13" s="10" customFormat="1" ht="406" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="77" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="60">
-        <v>2</v>
-      </c>
-      <c r="C4" s="61" t="s">
-        <v>49</v>
-      </c>
-      <c r="D4" s="62" t="s">
-        <v>54</v>
-      </c>
-      <c r="E4" s="62" t="s">
+      <c r="F5" s="75" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="93" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="93"/>
+      <c r="I5" s="94"/>
+      <c r="J5" s="76" t="s">
+        <v>12</v>
+      </c>
+      <c r="K5" s="94" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="62" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" s="63" t="s">
-        <v>32</v>
-      </c>
-      <c r="H4" s="64" t="s">
-        <v>43</v>
-      </c>
-      <c r="I4" s="65" t="s">
-        <v>34</v>
-      </c>
-      <c r="J4" s="62" t="s">
-        <v>9</v>
-      </c>
-      <c r="K4" s="82" t="s">
-        <v>24</v>
-      </c>
-      <c r="L4" s="83"/>
-      <c r="M4" s="6"/>
-    </row>
-    <row r="5" spans="1:13" s="11" customFormat="1" ht="343" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="77"/>
-      <c r="B5" s="50">
-        <v>3</v>
-      </c>
-      <c r="C5" s="51" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="52" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="52" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="52" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5" s="78" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" s="78"/>
-      <c r="I5" s="79"/>
-      <c r="J5" s="53" t="s">
-        <v>12</v>
-      </c>
-      <c r="K5" s="79" t="s">
-        <v>23</v>
-      </c>
-      <c r="L5" s="84"/>
+      <c r="L5" s="99"/>
       <c r="M5" s="7"/>
     </row>
-    <row r="6" spans="1:13" s="49" customFormat="1" ht="100" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="75" t="s">
-        <v>46</v>
-      </c>
-      <c r="B6" s="75"/>
-      <c r="C6" s="75"/>
-      <c r="D6" s="75"/>
-      <c r="E6" s="75"/>
-      <c r="F6" s="75"/>
-      <c r="G6" s="75"/>
-      <c r="H6" s="75"/>
-      <c r="I6" s="75"/>
-      <c r="J6" s="75"/>
-      <c r="K6" s="75"/>
-      <c r="L6" s="75"/>
+    <row r="6" spans="1:13" s="42" customFormat="1" ht="100" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="90" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="90"/>
+      <c r="C6" s="90"/>
+      <c r="D6" s="90"/>
+      <c r="E6" s="90"/>
+      <c r="F6" s="90"/>
+      <c r="G6" s="90"/>
+      <c r="H6" s="90"/>
+      <c r="I6" s="90"/>
+      <c r="J6" s="90"/>
+      <c r="K6" s="90"/>
+      <c r="L6" s="90"/>
     </row>
     <row r="7" spans="1:13" ht="30" thickTop="1" x14ac:dyDescent="0.35"/>
     <row r="10" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="C10" s="47"/>
+      <c r="C10" s="40"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="C11" s="48"/>
+      <c r="C11" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -1704,10 +1938,10 @@
     <tabColor theme="8" tint="0.79998168889431442"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView zoomScale="36" zoomScaleNormal="89" zoomScalePageLayoutView="50" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView zoomScale="50" zoomScaleNormal="58" zoomScalePageLayoutView="50" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="29" x14ac:dyDescent="0.35"/>
@@ -1717,165 +1951,150 @@
     <col min="3" max="3" width="35.5" style="4" customWidth="1"/>
     <col min="4" max="4" width="48" style="13" customWidth="1"/>
     <col min="5" max="5" width="62.6640625" style="13" customWidth="1"/>
-    <col min="6" max="6" width="33" style="13" customWidth="1"/>
-    <col min="7" max="7" width="39.6640625" style="14" customWidth="1"/>
+    <col min="6" max="6" width="36.33203125" style="13" customWidth="1"/>
+    <col min="7" max="7" width="34" style="14" customWidth="1"/>
     <col min="8" max="8" width="63.5" style="14" customWidth="1"/>
     <col min="9" max="9" width="63.5" style="13" customWidth="1"/>
     <col min="10" max="10" width="36.1640625" style="13" customWidth="1"/>
     <col min="11" max="16384" width="10.83203125" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="43" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="88" t="s">
+    <row r="1" spans="1:11" s="20" customFormat="1" ht="80" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="19"/>
+    </row>
+    <row r="2" spans="1:11" s="9" customFormat="1" ht="284" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="24">
+        <v>1</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="77" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="77" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="78" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" s="79" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" s="79" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" s="79" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" s="77" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" s="12"/>
+    </row>
+    <row r="3" spans="1:11" s="10" customFormat="1" ht="329" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="92" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="49">
+        <v>2</v>
+      </c>
+      <c r="C3" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="88"/>
-      <c r="C1" s="88"/>
-      <c r="D1" s="88"/>
-      <c r="E1" s="88"/>
-      <c r="F1" s="88"/>
-      <c r="G1" s="88"/>
-      <c r="H1" s="88"/>
-      <c r="I1" s="88"/>
-      <c r="J1" s="88"/>
-    </row>
-    <row r="2" spans="1:11" s="21" customFormat="1" ht="80" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="38" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="39" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="40" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="41" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="41" t="s">
-        <v>40</v>
-      </c>
-      <c r="F2" s="46" t="s">
-        <v>2</v>
-      </c>
-      <c r="G2" s="41" t="s">
+      <c r="D3" s="80" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" s="80" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" s="80" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="81" t="s">
         <v>29</v>
       </c>
-      <c r="H2" s="41" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" s="41" t="s">
-        <v>10</v>
-      </c>
-      <c r="J2" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="K2" s="20"/>
-    </row>
-    <row r="3" spans="1:11" s="9" customFormat="1" ht="272" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="26">
-        <v>1</v>
-      </c>
-      <c r="C3" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="28" t="s">
+      <c r="H3" s="82" t="s">
+        <v>38</v>
+      </c>
+      <c r="I3" s="83" t="s">
+        <v>31</v>
+      </c>
+      <c r="J3" s="84" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" s="6"/>
+    </row>
+    <row r="4" spans="1:11" s="11" customFormat="1" ht="220" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="100"/>
+      <c r="B4" s="17">
+        <v>3</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="85" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="28" t="s">
-        <v>50</v>
-      </c>
-      <c r="F3" s="33" t="s">
+      <c r="E4" s="85" t="s">
         <v>51</v>
       </c>
-      <c r="G3" s="29" t="s">
-        <v>31</v>
-      </c>
-      <c r="H3" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="I3" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="J3" s="28" t="s">
+      <c r="F4" s="85" t="s">
         <v>25</v>
       </c>
-      <c r="K3" s="12"/>
-    </row>
-    <row r="4" spans="1:11" s="10" customFormat="1" ht="359" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="77" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="60">
-        <v>2</v>
-      </c>
-      <c r="C4" s="66" t="s">
-        <v>52</v>
-      </c>
-      <c r="D4" s="67" t="s">
-        <v>54</v>
-      </c>
-      <c r="E4" s="67" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="67" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" s="68" t="s">
-        <v>32</v>
-      </c>
-      <c r="H4" s="69" t="s">
-        <v>43</v>
-      </c>
-      <c r="I4" s="70" t="s">
-        <v>34</v>
-      </c>
-      <c r="J4" s="71" t="s">
-        <v>26</v>
-      </c>
-      <c r="K4" s="6"/>
-    </row>
-    <row r="5" spans="1:11" s="11" customFormat="1" ht="252" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="85"/>
-      <c r="B5" s="17">
-        <v>3</v>
-      </c>
-      <c r="C5" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5" s="86" t="s">
-        <v>38</v>
-      </c>
-      <c r="H5" s="86"/>
-      <c r="I5" s="87"/>
-      <c r="J5" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="K5" s="7"/>
-    </row>
-    <row r="6" spans="1:11" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="2"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="15"/>
-      <c r="I6" s="16"/>
+      <c r="G4" s="101" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" s="101"/>
+      <c r="I4" s="102"/>
+      <c r="J4" s="86" t="s">
+        <v>24</v>
+      </c>
+      <c r="K4" s="7"/>
+    </row>
+    <row r="5" spans="1:11" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="2"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="15"/>
+      <c r="I5" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="A1:J1"/>
+  <mergeCells count="2">
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="G4:I4"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup scale="28" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1890,8 +2109,8 @@
   </sheetPr>
   <dimension ref="A2:I6"/>
   <sheetViews>
-    <sheetView zoomScale="56" zoomScaleNormal="72" zoomScalePageLayoutView="50" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView topLeftCell="A3" zoomScale="56" zoomScaleNormal="72" zoomScalePageLayoutView="50" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="29" x14ac:dyDescent="0.35"/>
@@ -1902,111 +2121,111 @@
     <col min="4" max="4" width="48" style="13" customWidth="1"/>
     <col min="5" max="5" width="54.5" style="13" customWidth="1"/>
     <col min="6" max="6" width="35.1640625" style="13" customWidth="1"/>
-    <col min="7" max="7" width="69.83203125" style="8" customWidth="1"/>
+    <col min="7" max="7" width="87.33203125" style="8" customWidth="1"/>
     <col min="8" max="8" width="33.1640625" style="13" customWidth="1"/>
     <col min="9" max="16384" width="10.83203125" style="8"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" s="21" customFormat="1" ht="107" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="38" t="s">
+    <row r="2" spans="1:9" s="20" customFormat="1" ht="107" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="40" t="s">
+      <c r="C2" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="41" t="s">
+      <c r="D2" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="41" t="s">
-        <v>40</v>
-      </c>
-      <c r="F2" s="41" t="s">
+      <c r="E2" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="41" t="s">
-        <v>37</v>
-      </c>
-      <c r="H2" s="41" t="s">
+      <c r="G2" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" s="34" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="9" customFormat="1" ht="242" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="26">
+      <c r="B3" s="24">
         <v>1</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="34" t="s">
-        <v>41</v>
-      </c>
-      <c r="E3" s="34" t="s">
+      <c r="E3" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="G3" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" s="27" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="10" customFormat="1" ht="313" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="92" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="49">
+        <v>2</v>
+      </c>
+      <c r="C4" s="51" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="52" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" s="52" t="s">
         <v>50</v>
       </c>
-      <c r="F3" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="G3" s="34" t="s">
+      <c r="F4" s="52" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="53" t="s">
         <v>39</v>
       </c>
-      <c r="H3" s="34" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" s="10" customFormat="1" ht="370" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="77" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="60">
-        <v>2</v>
-      </c>
-      <c r="C4" s="66" t="s">
-        <v>49</v>
-      </c>
-      <c r="D4" s="72" t="s">
-        <v>54</v>
-      </c>
-      <c r="E4" s="72" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="72" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" s="73" t="s">
-        <v>44</v>
-      </c>
-      <c r="H4" s="73" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" s="11" customFormat="1" ht="158" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="85"/>
+      <c r="H4" s="53" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="11" customFormat="1" ht="201" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="100"/>
       <c r="B5" s="17">
         <v>3</v>
       </c>
       <c r="C5" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="36" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="36" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="36" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5" s="35" t="s">
-        <v>38</v>
-      </c>
-      <c r="H5" s="37" t="s">
-        <v>27</v>
+      <c r="D5" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" s="29" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="H5" s="30" t="s">
+        <v>24</v>
       </c>
       <c r="I5"/>
     </row>
@@ -2025,6 +2244,121 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0FCFCAA-08C9-2F49-B7A3-F3DED9B06E31}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="4.5" style="68" customWidth="1"/>
+    <col min="3" max="3" width="25.6640625" style="4" customWidth="1"/>
+    <col min="4" max="5" width="37.33203125" style="4" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="35" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="103" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="103"/>
+      <c r="C1" s="103"/>
+      <c r="D1" s="103"/>
+      <c r="E1" s="103"/>
+    </row>
+    <row r="2" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="54" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="55" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="54" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="54" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="54" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="60" customFormat="1" ht="100" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="56" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="57">
+        <v>1</v>
+      </c>
+      <c r="C3" s="58" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" s="59" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="60" customFormat="1" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="104" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="61">
+        <v>2</v>
+      </c>
+      <c r="C4" s="62" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="63" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" s="63" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="60" customFormat="1" ht="100" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="105"/>
+      <c r="B5" s="64">
+        <v>3</v>
+      </c>
+      <c r="C5" s="65" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="66" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="66" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="67" customFormat="1" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="106" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="107"/>
+      <c r="C6" s="107"/>
+      <c r="D6" s="107"/>
+      <c r="E6" s="107"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A6:E6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{622BE0EC-7840-5D46-A8D2-9418A2D8E32D}">
   <sheetPr>
     <tabColor theme="8" tint="0.79998168889431442"/>
@@ -2032,47 +2366,47 @@
   </sheetPr>
   <dimension ref="A2:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="125" zoomScalePageLayoutView="50" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScale="131" zoomScaleNormal="131" zoomScalePageLayoutView="50" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17" style="1" customWidth="1"/>
-    <col min="2" max="2" width="103.6640625" style="13" customWidth="1"/>
+    <col min="2" max="2" width="99.6640625" style="13" customWidth="1"/>
     <col min="3" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" s="59" customFormat="1" ht="37" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="39" t="s">
+    <row r="2" spans="1:3" s="48" customFormat="1" ht="37" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="33" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="132" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="58">
+    <row r="3" spans="1:3" ht="151" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="47">
         <v>1</v>
       </c>
-      <c r="B3" s="57" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" s="56" customFormat="1" ht="130" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="60">
+      <c r="B3" s="87" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="46" customFormat="1" ht="100" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="49">
         <v>2</v>
       </c>
-      <c r="B4" s="74" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" s="54" customFormat="1" ht="99" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="88" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="45" customFormat="1" ht="99" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="17">
         <v>3</v>
       </c>
-      <c r="B5" s="55" t="s">
-        <v>47</v>
+      <c r="B5" s="89" t="s">
+        <v>56</v>
       </c>
       <c r="C5"/>
     </row>
@@ -2082,6 +2416,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup scale="37" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup scale="97" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
 </file>
</xml_diff>